<commit_message>
add validation in master fleet
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/masterFleet.xlsx
+++ b/FMS.Website/files_upload/masterFleet.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vox\task\fms021020170830\hms-fms\FMS.Website\files_upload\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AV$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AW$52</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -22,7 +27,7 @@
     <author>Gani, Ida</author>
   </authors>
   <commentList>
-    <comment ref="V3" authorId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0">
+    <comment ref="AA3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +71,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="0">
+    <comment ref="AB3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Gani, Ida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+data dari master data price list</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH3" authorId="0">
+    <comment ref="AI3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP3" authorId="0">
+    <comment ref="AQ3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ3" authorId="0">
+    <comment ref="AR3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="402">
   <si>
     <t>MASTER DATA FLEET</t>
   </si>
@@ -1363,21 +1390,21 @@
   </si>
   <si>
     <t>22.01.14 Ex. AME/SAM ; 25.09.13 Email Pebri (TRAC) info nopol barunya (ex. AB1872X).</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1394,22 +1421,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1418,134 +1429,17 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1558,194 +1452,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1753,320 +1461,38 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2324,52 +1750,51 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:AV52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="1" ySplit="3" topLeftCell="T16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="16" max="16" width="10.8571428571429" customWidth="1"/>
-    <col min="17" max="17" width="14.4285714285714" customWidth="1"/>
-    <col min="18" max="20" width="19.1428571428571" customWidth="1"/>
-    <col min="23" max="25" width="8.71428571428571" customWidth="1"/>
-    <col min="27" max="27" width="13.5714285714286" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5714285714286" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="31" width="8.71428571428571" customWidth="1"/>
-    <col min="32" max="32" width="11.7142857142857" customWidth="1"/>
-    <col min="33" max="33" width="15.4285714285714" customWidth="1"/>
-    <col min="34" max="36" width="9.85714285714286" style="2" customWidth="1"/>
-    <col min="37" max="37" width="18" customWidth="1"/>
-    <col min="39" max="40" width="8.71428571428571" customWidth="1"/>
-    <col min="41" max="41" width="19" style="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5714285714286" customWidth="1"/>
-    <col min="43" max="43" width="13.5714285714286" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="18" max="20" width="19.140625" customWidth="1"/>
+    <col min="23" max="25" width="8.7109375" customWidth="1"/>
+    <col min="27" max="28" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="11" customWidth="1"/>
+    <col min="31" max="32" width="8.7109375" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" customWidth="1"/>
+    <col min="35" max="37" width="9.85546875" style="2" customWidth="1"/>
+    <col min="38" max="38" width="18" customWidth="1"/>
+    <col min="40" max="41" width="8.7109375" customWidth="1"/>
+    <col min="42" max="42" width="19" style="1" customWidth="1"/>
+    <col min="43" max="43" width="14.5703125" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:49">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customHeight="1"/>
-    <row r="3" spans="1:48">
+    <row r="2" spans="1:49" ht="15" customHeight="1"/>
+    <row r="3" spans="1:49">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2452,70 +1877,73 @@
         <v>27</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AI3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>37</v>
       </c>
-      <c r="AL3" s="7" t="s">
+      <c r="AM3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AM3" s="7" t="s">
+      <c r="AN3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AN3" s="7" t="s">
+      <c r="AO3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AO3" s="9" t="s">
+      <c r="AP3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AQ3" s="10" t="s">
+      <c r="AR3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AU3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AW3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:49">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2592,41 +2020,44 @@
         <v>7680000</v>
       </c>
       <c r="AB4" s="1">
+        <v>7680000</v>
+      </c>
+      <c r="AC4" s="1">
         <v>768000</v>
       </c>
-      <c r="AC4" s="5">
+      <c r="AD4" s="5">
         <v>4500582129</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>70</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>2</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AJ4" s="2">
         <v>41379</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AK4" s="2">
         <v>43204</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>71</v>
       </c>
-      <c r="AL4" t="s">
-        <v>72</v>
-      </c>
       <c r="AM4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN4" t="s">
         <v>73</v>
       </c>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="1">
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="1">
         <v>8448000</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:49">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2703,41 +2134,44 @@
         <v>5599000</v>
       </c>
       <c r="AB5" s="1">
+        <v>5599000</v>
+      </c>
+      <c r="AC5" s="1">
         <v>559900</v>
       </c>
-      <c r="AC5" s="5">
+      <c r="AD5" s="5">
         <v>4500649197</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>70</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>1</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AJ5" s="2">
         <v>41487</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AK5" s="2">
         <v>43312</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>71</v>
       </c>
-      <c r="AL5" t="s">
-        <v>72</v>
-      </c>
       <c r="AM5" t="s">
         <v>72</v>
       </c>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="1">
+      <c r="AN5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="1">
         <v>6158900</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:49">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -2808,44 +2242,47 @@
         <v>8050000</v>
       </c>
       <c r="AB6" s="1">
+        <v>8050000</v>
+      </c>
+      <c r="AC6" s="1">
         <v>805000</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AD6" s="5">
         <v>4501334986</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>70</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>1</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AJ6" s="2">
         <v>43009</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AK6" s="2">
         <v>44834</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>71</v>
       </c>
-      <c r="AL6" t="s">
-        <v>72</v>
-      </c>
       <c r="AM6" t="s">
         <v>72</v>
       </c>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="1">
+      <c r="AN6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="1">
         <v>8855000</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>95</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:49">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -2916,47 +2353,50 @@
         <v>2890000</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="5">
         <v>4500705483</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>70</v>
       </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="s">
         <v>98</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AJ7" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="AK7" s="2">
         <v>43465</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>71</v>
       </c>
-      <c r="AL7" t="s">
-        <v>72</v>
-      </c>
       <c r="AM7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN7" t="s">
         <v>111</v>
       </c>
-      <c r="AN7" s="8"/>
-      <c r="AO7" s="1">
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>95</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:49">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -3027,47 +2467,50 @@
         <v>2890000</v>
       </c>
       <c r="AB8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="5">
         <v>4500705432</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>120</v>
       </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s">
         <v>113</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AJ8" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="AK8" s="2">
         <v>43465</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AL8" t="s">
         <v>71</v>
       </c>
-      <c r="AL8" t="s">
-        <v>72</v>
-      </c>
       <c r="AM8" t="s">
         <v>72</v>
       </c>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="1">
+      <c r="AN8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AQ8" t="s">
         <v>95</v>
       </c>
-      <c r="AQ8" t="s">
+      <c r="AR8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:49">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3138,47 +2581,50 @@
         <v>2890000</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="5">
         <v>4500705635</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>70</v>
       </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AG9" t="s">
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="s">
         <v>122</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="AJ9" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ9" s="2">
+      <c r="AK9" s="2">
         <v>43465</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>71</v>
       </c>
-      <c r="AL9" t="s">
-        <v>72</v>
-      </c>
       <c r="AM9" t="s">
         <v>72</v>
       </c>
-      <c r="AN9" s="8"/>
-      <c r="AO9" s="1">
+      <c r="AN9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>95</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AR9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:49">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -3249,47 +2695,50 @@
         <v>2890000</v>
       </c>
       <c r="AB10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="5">
         <v>4500705467</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>120</v>
       </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AG10" t="s">
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="s">
         <v>130</v>
       </c>
-      <c r="AI10" s="2">
+      <c r="AJ10" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ10" s="2">
+      <c r="AK10" s="2">
         <v>43465</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>71</v>
       </c>
-      <c r="AL10" t="s">
-        <v>72</v>
-      </c>
       <c r="AM10" t="s">
         <v>72</v>
       </c>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="1">
+      <c r="AN10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AQ10" t="s">
         <v>95</v>
       </c>
-      <c r="AQ10" t="s">
+      <c r="AR10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:49">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -3360,47 +2809,50 @@
         <v>2890000</v>
       </c>
       <c r="AB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="5">
         <v>4500705640</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>70</v>
       </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="s">
         <v>138</v>
       </c>
-      <c r="AI11" s="2">
+      <c r="AJ11" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ11" s="2">
+      <c r="AK11" s="2">
         <v>43465</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AL11" t="s">
         <v>71</v>
       </c>
-      <c r="AL11" t="s">
-        <v>72</v>
-      </c>
       <c r="AM11" t="s">
         <v>72</v>
       </c>
-      <c r="AN11" s="8"/>
-      <c r="AO11" s="1">
+      <c r="AN11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AQ11" t="s">
         <v>95</v>
       </c>
-      <c r="AQ11" t="s">
+      <c r="AR11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:49">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -3471,47 +2923,50 @@
         <v>2890000</v>
       </c>
       <c r="AB12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="5">
         <v>4500705478</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>120</v>
       </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AG12" t="s">
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="s">
         <v>143</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AJ12" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ12" s="2">
+      <c r="AK12" s="2">
         <v>43465</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
         <v>71</v>
       </c>
-      <c r="AL12" t="s">
-        <v>72</v>
-      </c>
       <c r="AM12" t="s">
         <v>72</v>
       </c>
-      <c r="AN12" s="8"/>
-      <c r="AO12" s="1">
+      <c r="AN12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP12" t="s">
+      <c r="AQ12" t="s">
         <v>95</v>
       </c>
-      <c r="AQ12" t="s">
+      <c r="AR12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:49">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -3582,47 +3037,50 @@
         <v>2890000</v>
       </c>
       <c r="AB13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="5">
         <v>4500705478</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>70</v>
       </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AG13" t="s">
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="s">
         <v>149</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AJ13" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="AK13" s="2">
         <v>43465</v>
       </c>
-      <c r="AK13" t="s">
+      <c r="AL13" t="s">
         <v>71</v>
       </c>
-      <c r="AL13" t="s">
-        <v>72</v>
-      </c>
       <c r="AM13" t="s">
         <v>72</v>
       </c>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="1">
+      <c r="AN13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP13" t="s">
+      <c r="AQ13" t="s">
         <v>95</v>
       </c>
-      <c r="AQ13" t="s">
+      <c r="AR13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:49">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -3693,47 +3151,50 @@
         <v>3060000</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="5">
         <v>4500780545</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>120</v>
       </c>
-      <c r="AE14">
-        <v>0</v>
-      </c>
-      <c r="AG14" t="s">
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="s">
         <v>154</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="AJ14" s="2">
         <v>41744</v>
       </c>
-      <c r="AJ14" s="2">
+      <c r="AK14" s="2">
         <v>43569</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AL14" t="s">
         <v>71</v>
       </c>
-      <c r="AL14" t="s">
-        <v>72</v>
-      </c>
       <c r="AM14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN14" t="s">
         <v>160</v>
       </c>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="1">
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP14" t="s">
+      <c r="AQ14" t="s">
         <v>95</v>
       </c>
-      <c r="AQ14" t="s">
+      <c r="AR14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:49">
       <c r="A15" t="s">
         <v>161</v>
       </c>
@@ -3804,47 +3265,50 @@
         <v>2890000</v>
       </c>
       <c r="AB15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="5">
         <v>4500705432</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>70</v>
       </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AG15" t="s">
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AH15" t="s">
         <v>162</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AJ15" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AK15" s="2">
         <v>43465</v>
       </c>
-      <c r="AK15" t="s">
+      <c r="AL15" t="s">
         <v>71</v>
       </c>
-      <c r="AL15" t="s">
-        <v>72</v>
-      </c>
       <c r="AM15" t="s">
         <v>72</v>
       </c>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="1">
+      <c r="AN15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO15" s="8"/>
+      <c r="AP15" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP15" t="s">
+      <c r="AQ15" t="s">
         <v>95</v>
       </c>
-      <c r="AQ15" t="s">
+      <c r="AR15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:49">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -3915,41 +3379,44 @@
         <v>5459900</v>
       </c>
       <c r="AB16" s="1">
+        <v>5459900</v>
+      </c>
+      <c r="AC16" s="1">
         <v>545990</v>
       </c>
-      <c r="AC16" s="5">
+      <c r="AD16" s="5">
         <v>4500751694</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>176</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>1</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AJ16" s="2">
         <v>41518</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="AK16" s="2">
         <v>43343</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AL16" t="s">
         <v>71</v>
       </c>
-      <c r="AL16" t="s">
-        <v>72</v>
-      </c>
       <c r="AM16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN16" t="s">
         <v>177</v>
       </c>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="1">
+      <c r="AO16" s="8"/>
+      <c r="AP16" s="1">
         <v>6005890</v>
       </c>
-      <c r="AP16" t="s">
+      <c r="AQ16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:44">
       <c r="A17" t="s">
         <v>178</v>
       </c>
@@ -4020,47 +3487,50 @@
         <v>3520000</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="5">
+        <v>3520000</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="5">
         <v>4501121841</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>70</v>
       </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
-      <c r="AG17" t="s">
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="s">
         <v>179</v>
       </c>
-      <c r="AI17" s="2">
+      <c r="AJ17" s="2">
         <v>42491</v>
       </c>
-      <c r="AJ17" s="2">
+      <c r="AK17" s="2">
         <v>44316</v>
       </c>
-      <c r="AK17" t="s">
+      <c r="AL17" t="s">
         <v>71</v>
       </c>
-      <c r="AL17" t="s">
-        <v>72</v>
-      </c>
       <c r="AM17" t="s">
         <v>72</v>
       </c>
-      <c r="AN17" s="8"/>
-      <c r="AO17" s="1">
+      <c r="AN17" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO17" s="8"/>
+      <c r="AP17" s="1">
         <v>3520000</v>
       </c>
-      <c r="AP17" t="s">
+      <c r="AQ17" t="s">
         <v>95</v>
       </c>
-      <c r="AQ17" t="s">
+      <c r="AR17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:44">
       <c r="A18" t="s">
         <v>187</v>
       </c>
@@ -4131,43 +3601,46 @@
         <v>17360000</v>
       </c>
       <c r="AB18" s="1">
+        <v>17360000</v>
+      </c>
+      <c r="AC18" s="1">
         <v>1736000</v>
       </c>
-      <c r="AC18" s="5">
+      <c r="AD18" s="5">
         <v>4500881617</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>70</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <v>3</v>
       </c>
-      <c r="AI18" s="2">
+      <c r="AJ18" s="2">
         <v>41958</v>
       </c>
-      <c r="AJ18" s="2">
+      <c r="AK18" s="2">
         <v>43783</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AL18" t="s">
         <v>71</v>
       </c>
-      <c r="AL18" t="s">
-        <v>72</v>
-      </c>
       <c r="AM18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN18" t="s">
         <v>197</v>
       </c>
-      <c r="AN18" s="8">
+      <c r="AO18" s="8">
         <v>701994</v>
       </c>
-      <c r="AO18" s="1">
+      <c r="AP18" s="1">
         <v>19096000</v>
       </c>
-      <c r="AP18" t="s">
+      <c r="AQ18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:44">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -4238,41 +3711,44 @@
         <v>6254000</v>
       </c>
       <c r="AB19" s="1">
+        <v>6254000</v>
+      </c>
+      <c r="AC19" s="1">
         <v>625400</v>
       </c>
-      <c r="AC19" s="5">
+      <c r="AD19" s="5">
         <v>4500862592</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>70</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>1</v>
       </c>
-      <c r="AI19" s="2">
+      <c r="AJ19" s="2">
         <v>41927</v>
       </c>
-      <c r="AJ19" s="2">
+      <c r="AK19" s="2">
         <v>43752</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AL19" t="s">
         <v>71</v>
       </c>
-      <c r="AL19" t="s">
-        <v>72</v>
-      </c>
       <c r="AM19" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN19" t="s">
         <v>205</v>
       </c>
-      <c r="AN19" s="8"/>
-      <c r="AO19" s="1">
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="1">
         <v>6879400</v>
       </c>
-      <c r="AP19" t="s">
+      <c r="AQ19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:44">
       <c r="A20" t="s">
         <v>206</v>
       </c>
@@ -4343,47 +3819,50 @@
         <v>3060000</v>
       </c>
       <c r="AB20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="5">
         <v>4500812381</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>120</v>
       </c>
-      <c r="AE20">
-        <v>0</v>
-      </c>
-      <c r="AG20" t="s">
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AH20" t="s">
         <v>207</v>
       </c>
-      <c r="AI20" s="2">
+      <c r="AJ20" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ20" s="2">
+      <c r="AK20" s="2">
         <v>43630</v>
       </c>
-      <c r="AK20" t="s">
+      <c r="AL20" t="s">
         <v>71</v>
       </c>
-      <c r="AL20" t="s">
-        <v>72</v>
-      </c>
       <c r="AM20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN20" t="s">
         <v>212</v>
       </c>
-      <c r="AN20" s="8"/>
-      <c r="AO20" s="1">
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP20" t="s">
+      <c r="AQ20" t="s">
         <v>95</v>
       </c>
-      <c r="AQ20" t="s">
+      <c r="AR20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:44">
       <c r="A21" t="s">
         <v>213</v>
       </c>
@@ -4454,47 +3933,50 @@
         <v>3060000</v>
       </c>
       <c r="AB21" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="5">
         <v>4500812540</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>70</v>
       </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
-      <c r="AG21" t="s">
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AH21" t="s">
         <v>214</v>
       </c>
-      <c r="AI21" s="2">
+      <c r="AJ21" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ21" s="2">
+      <c r="AK21" s="2">
         <v>43630</v>
       </c>
-      <c r="AK21" t="s">
+      <c r="AL21" t="s">
         <v>71</v>
       </c>
-      <c r="AL21" t="s">
-        <v>72</v>
-      </c>
       <c r="AM21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN21" t="s">
         <v>218</v>
       </c>
-      <c r="AN21" s="8"/>
-      <c r="AO21" s="1">
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP21" t="s">
+      <c r="AQ21" t="s">
         <v>95</v>
       </c>
-      <c r="AQ21" t="s">
+      <c r="AR21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:44">
       <c r="A22" t="s">
         <v>219</v>
       </c>
@@ -4565,47 +4047,50 @@
         <v>3060000</v>
       </c>
       <c r="AB22" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="5">
         <v>4500812381</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>70</v>
       </c>
-      <c r="AE22">
-        <v>0</v>
-      </c>
-      <c r="AG22" t="s">
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AH22" t="s">
         <v>220</v>
       </c>
-      <c r="AI22" s="2">
+      <c r="AJ22" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ22" s="2">
+      <c r="AK22" s="2">
         <v>43630</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AL22" t="s">
         <v>71</v>
       </c>
-      <c r="AL22" t="s">
-        <v>72</v>
-      </c>
       <c r="AM22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN22" t="s">
         <v>224</v>
       </c>
-      <c r="AN22" s="8"/>
-      <c r="AO22" s="1">
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP22" t="s">
+      <c r="AQ22" t="s">
         <v>95</v>
       </c>
-      <c r="AQ22" t="s">
+      <c r="AR22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:44">
       <c r="A23" t="s">
         <v>225</v>
       </c>
@@ -4676,47 +4161,50 @@
         <v>3060000</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="5">
         <v>4500812457</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>120</v>
       </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="s">
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AH23" t="s">
         <v>226</v>
       </c>
-      <c r="AI23" s="2">
+      <c r="AJ23" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ23" s="2">
+      <c r="AK23" s="2">
         <v>43630</v>
       </c>
-      <c r="AK23" t="s">
+      <c r="AL23" t="s">
         <v>71</v>
       </c>
-      <c r="AL23" t="s">
-        <v>72</v>
-      </c>
       <c r="AM23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN23" t="s">
         <v>232</v>
       </c>
-      <c r="AN23" s="8"/>
-      <c r="AO23" s="1">
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP23" t="s">
+      <c r="AQ23" t="s">
         <v>95</v>
       </c>
-      <c r="AQ23" t="s">
+      <c r="AR23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:44">
       <c r="A24" t="s">
         <v>233</v>
       </c>
@@ -4787,47 +4275,50 @@
         <v>3060000</v>
       </c>
       <c r="AB24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="5">
         <v>4500812456</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>70</v>
       </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-      <c r="AG24" t="s">
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AH24" t="s">
         <v>234</v>
       </c>
-      <c r="AI24" s="2">
+      <c r="AJ24" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ24" s="2">
+      <c r="AK24" s="2">
         <v>43630</v>
       </c>
-      <c r="AK24" t="s">
+      <c r="AL24" t="s">
         <v>71</v>
       </c>
-      <c r="AL24" t="s">
-        <v>72</v>
-      </c>
       <c r="AM24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN24" t="s">
         <v>238</v>
       </c>
-      <c r="AN24" s="8"/>
-      <c r="AO24" s="1">
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP24" t="s">
+      <c r="AQ24" t="s">
         <v>95</v>
       </c>
-      <c r="AQ24" t="s">
+      <c r="AR24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:44">
       <c r="A25" t="s">
         <v>239</v>
       </c>
@@ -4898,47 +4389,50 @@
         <v>3060000</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="5">
         <v>4500812376</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>70</v>
       </c>
-      <c r="AE25">
-        <v>0</v>
-      </c>
-      <c r="AG25" t="s">
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="s">
         <v>240</v>
       </c>
-      <c r="AI25" s="2">
+      <c r="AJ25" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ25" s="2">
+      <c r="AK25" s="2">
         <v>43630</v>
       </c>
-      <c r="AK25" t="s">
+      <c r="AL25" t="s">
         <v>71</v>
       </c>
-      <c r="AL25" t="s">
-        <v>72</v>
-      </c>
       <c r="AM25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN25" t="s">
         <v>244</v>
       </c>
-      <c r="AN25" s="8"/>
-      <c r="AO25" s="1">
+      <c r="AO25" s="8"/>
+      <c r="AP25" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP25" t="s">
+      <c r="AQ25" t="s">
         <v>95</v>
       </c>
-      <c r="AQ25" t="s">
+      <c r="AR25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:44">
       <c r="A26" t="s">
         <v>245</v>
       </c>
@@ -5009,47 +4503,50 @@
         <v>3060000</v>
       </c>
       <c r="AB26" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="5">
         <v>4500812457</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>250</v>
       </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-      <c r="AG26" t="s">
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AH26" t="s">
         <v>246</v>
       </c>
-      <c r="AI26" s="2">
+      <c r="AJ26" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ26" s="2">
+      <c r="AK26" s="2">
         <v>43630</v>
       </c>
-      <c r="AK26" t="s">
+      <c r="AL26" t="s">
         <v>71</v>
       </c>
-      <c r="AL26" t="s">
-        <v>72</v>
-      </c>
       <c r="AM26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN26" t="s">
         <v>251</v>
       </c>
-      <c r="AN26" s="8"/>
-      <c r="AO26" s="1">
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP26" t="s">
+      <c r="AQ26" t="s">
         <v>95</v>
       </c>
-      <c r="AQ26" t="s">
+      <c r="AR26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:44">
       <c r="A27" t="s">
         <v>252</v>
       </c>
@@ -5120,47 +4617,50 @@
         <v>3060000</v>
       </c>
       <c r="AB27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="5">
         <v>4500812457</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>70</v>
       </c>
-      <c r="AE27">
-        <v>0</v>
-      </c>
-      <c r="AG27" t="s">
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AH27" t="s">
         <v>253</v>
       </c>
-      <c r="AI27" s="2">
+      <c r="AJ27" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ27" s="2">
+      <c r="AK27" s="2">
         <v>43630</v>
       </c>
-      <c r="AK27" t="s">
+      <c r="AL27" t="s">
         <v>71</v>
       </c>
-      <c r="AL27" t="s">
-        <v>72</v>
-      </c>
       <c r="AM27" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN27" t="s">
         <v>257</v>
       </c>
-      <c r="AN27" s="8"/>
-      <c r="AO27" s="1">
+      <c r="AO27" s="8"/>
+      <c r="AP27" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP27" t="s">
+      <c r="AQ27" t="s">
         <v>95</v>
       </c>
-      <c r="AQ27" t="s">
+      <c r="AR27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:44">
       <c r="A28" t="s">
         <v>258</v>
       </c>
@@ -5231,47 +4731,50 @@
         <v>3060000</v>
       </c>
       <c r="AB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="5">
         <v>4500812456</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AE28" t="s">
         <v>250</v>
       </c>
-      <c r="AE28">
-        <v>0</v>
-      </c>
-      <c r="AG28" t="s">
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AH28" t="s">
         <v>259</v>
       </c>
-      <c r="AI28" s="2">
+      <c r="AJ28" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ28" s="2">
+      <c r="AK28" s="2">
         <v>43630</v>
       </c>
-      <c r="AK28" t="s">
+      <c r="AL28" t="s">
         <v>71</v>
       </c>
-      <c r="AL28" t="s">
-        <v>72</v>
-      </c>
       <c r="AM28" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN28" t="s">
         <v>263</v>
       </c>
-      <c r="AN28" s="8"/>
-      <c r="AO28" s="1">
+      <c r="AO28" s="8"/>
+      <c r="AP28" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP28" t="s">
+      <c r="AQ28" t="s">
         <v>95</v>
       </c>
-      <c r="AQ28" t="s">
+      <c r="AR28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:44">
       <c r="A29" t="s">
         <v>264</v>
       </c>
@@ -5342,47 +4845,50 @@
         <v>3060000</v>
       </c>
       <c r="AB29" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="5">
         <v>4500815381</v>
       </c>
-      <c r="AD29" t="s">
+      <c r="AE29" t="s">
         <v>70</v>
       </c>
-      <c r="AE29">
-        <v>0</v>
-      </c>
-      <c r="AG29" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI29" s="2">
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ29" s="2">
         <v>41852</v>
       </c>
-      <c r="AJ29" s="2">
+      <c r="AK29" s="2">
         <v>43677</v>
       </c>
-      <c r="AK29" t="s">
+      <c r="AL29" t="s">
         <v>71</v>
       </c>
-      <c r="AL29" t="s">
-        <v>72</v>
-      </c>
       <c r="AM29" t="s">
         <v>72</v>
       </c>
-      <c r="AN29" s="8"/>
-      <c r="AO29" s="1">
+      <c r="AN29" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO29" s="8"/>
+      <c r="AP29" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP29" t="s">
+      <c r="AQ29" t="s">
         <v>95</v>
       </c>
-      <c r="AQ29" t="s">
+      <c r="AR29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:44">
       <c r="A30" t="s">
         <v>267</v>
       </c>
@@ -5453,47 +4959,50 @@
         <v>3060000</v>
       </c>
       <c r="AB30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="5">
+        <v>3060000</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="5">
         <v>4500812456</v>
       </c>
-      <c r="AD30" t="s">
+      <c r="AE30" t="s">
         <v>120</v>
       </c>
-      <c r="AE30">
-        <v>0</v>
-      </c>
-      <c r="AG30" t="s">
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AH30" t="s">
         <v>268</v>
       </c>
-      <c r="AI30" s="2">
+      <c r="AJ30" s="2">
         <v>41805</v>
       </c>
-      <c r="AJ30" s="2">
+      <c r="AK30" s="2">
         <v>43630</v>
       </c>
-      <c r="AK30" t="s">
+      <c r="AL30" t="s">
         <v>71</v>
       </c>
-      <c r="AL30" t="s">
-        <v>72</v>
-      </c>
       <c r="AM30" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN30" t="s">
         <v>272</v>
       </c>
-      <c r="AN30" s="8"/>
-      <c r="AO30" s="1">
+      <c r="AO30" s="8"/>
+      <c r="AP30" s="1">
         <v>3060000</v>
       </c>
-      <c r="AP30" t="s">
+      <c r="AQ30" t="s">
         <v>95</v>
       </c>
-      <c r="AQ30" t="s">
+      <c r="AR30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:44">
       <c r="A31" t="s">
         <v>273</v>
       </c>
@@ -5564,47 +5073,50 @@
         <v>3150000</v>
       </c>
       <c r="AB31" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="5">
         <v>4500992789</v>
       </c>
-      <c r="AD31" t="s">
+      <c r="AE31" t="s">
         <v>70</v>
       </c>
-      <c r="AE31">
-        <v>0</v>
-      </c>
-      <c r="AG31" t="s">
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AH31" t="s">
         <v>274</v>
       </c>
-      <c r="AI31" s="2">
+      <c r="AJ31" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ31" s="2">
+      <c r="AK31" s="2">
         <v>44135</v>
       </c>
-      <c r="AK31" t="s">
+      <c r="AL31" t="s">
         <v>71</v>
       </c>
-      <c r="AL31" t="s">
-        <v>72</v>
-      </c>
       <c r="AM31" t="s">
         <v>72</v>
       </c>
-      <c r="AN31" s="8"/>
-      <c r="AO31" s="1">
+      <c r="AN31" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO31" s="8"/>
+      <c r="AP31" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP31" t="s">
+      <c r="AQ31" t="s">
         <v>281</v>
       </c>
-      <c r="AQ31" t="s">
+      <c r="AR31" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:44">
       <c r="A32" t="s">
         <v>282</v>
       </c>
@@ -5675,47 +5187,50 @@
         <v>3150000</v>
       </c>
       <c r="AB32" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="5">
         <v>4500992789</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AE32" t="s">
         <v>120</v>
       </c>
-      <c r="AE32">
-        <v>0</v>
-      </c>
-      <c r="AG32" t="s">
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AH32" t="s">
         <v>283</v>
       </c>
-      <c r="AI32" s="2">
+      <c r="AJ32" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ32" s="2">
+      <c r="AK32" s="2">
         <v>44135</v>
       </c>
-      <c r="AK32" t="s">
+      <c r="AL32" t="s">
         <v>71</v>
       </c>
-      <c r="AL32" t="s">
-        <v>72</v>
-      </c>
       <c r="AM32" t="s">
         <v>72</v>
       </c>
-      <c r="AN32" s="8"/>
-      <c r="AO32" s="1">
+      <c r="AN32" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO32" s="8"/>
+      <c r="AP32" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP32" t="s">
+      <c r="AQ32" t="s">
         <v>281</v>
       </c>
-      <c r="AQ32" t="s">
+      <c r="AR32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:44">
       <c r="A33" t="s">
         <v>287</v>
       </c>
@@ -5786,47 +5301,50 @@
         <v>3150000</v>
       </c>
       <c r="AB33" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC33" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="5">
         <v>4500992785</v>
       </c>
-      <c r="AD33" t="s">
+      <c r="AE33" t="s">
         <v>70</v>
       </c>
-      <c r="AE33">
-        <v>0</v>
-      </c>
-      <c r="AG33" t="s">
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="s">
         <v>288</v>
       </c>
-      <c r="AI33" s="2">
+      <c r="AJ33" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ33" s="2">
+      <c r="AK33" s="2">
         <v>44135</v>
       </c>
-      <c r="AK33" t="s">
+      <c r="AL33" t="s">
         <v>71</v>
       </c>
-      <c r="AL33" t="s">
-        <v>72</v>
-      </c>
       <c r="AM33" t="s">
         <v>72</v>
       </c>
-      <c r="AN33" s="8"/>
-      <c r="AO33" s="1">
+      <c r="AN33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO33" s="8"/>
+      <c r="AP33" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP33" t="s">
+      <c r="AQ33" t="s">
         <v>281</v>
       </c>
-      <c r="AQ33" t="s">
+      <c r="AR33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:44">
       <c r="A34" t="s">
         <v>293</v>
       </c>
@@ -5897,47 +5415,50 @@
         <v>3150000</v>
       </c>
       <c r="AB34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="5">
         <v>4500992785</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AE34" t="s">
         <v>120</v>
       </c>
-      <c r="AE34">
-        <v>0</v>
-      </c>
-      <c r="AG34" t="s">
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="s">
         <v>294</v>
       </c>
-      <c r="AI34" s="2">
+      <c r="AJ34" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ34" s="2">
+      <c r="AK34" s="2">
         <v>44135</v>
       </c>
-      <c r="AK34" t="s">
+      <c r="AL34" t="s">
         <v>71</v>
       </c>
-      <c r="AL34" t="s">
-        <v>72</v>
-      </c>
       <c r="AM34" t="s">
         <v>72</v>
       </c>
-      <c r="AN34" s="8"/>
-      <c r="AO34" s="1">
+      <c r="AN34" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO34" s="8"/>
+      <c r="AP34" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP34" t="s">
+      <c r="AQ34" t="s">
         <v>281</v>
       </c>
-      <c r="AQ34" t="s">
+      <c r="AR34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:44">
       <c r="A35" t="s">
         <v>298</v>
       </c>
@@ -6008,47 +5529,50 @@
         <v>3150000</v>
       </c>
       <c r="AB35" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="5">
         <v>4500992785</v>
       </c>
-      <c r="AD35" t="s">
+      <c r="AE35" t="s">
         <v>250</v>
       </c>
-      <c r="AE35">
-        <v>0</v>
-      </c>
-      <c r="AG35" t="s">
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="s">
         <v>299</v>
       </c>
-      <c r="AI35" s="2">
+      <c r="AJ35" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ35" s="2">
+      <c r="AK35" s="2">
         <v>44135</v>
       </c>
-      <c r="AK35" t="s">
+      <c r="AL35" t="s">
         <v>71</v>
       </c>
-      <c r="AL35" t="s">
-        <v>72</v>
-      </c>
       <c r="AM35" t="s">
         <v>72</v>
       </c>
-      <c r="AN35" s="8"/>
-      <c r="AO35" s="1">
+      <c r="AN35" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO35" s="8"/>
+      <c r="AP35" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP35" t="s">
+      <c r="AQ35" t="s">
         <v>281</v>
       </c>
-      <c r="AQ35" t="s">
+      <c r="AR35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:44">
       <c r="A36" t="s">
         <v>303</v>
       </c>
@@ -6119,47 +5643,50 @@
         <v>3150000</v>
       </c>
       <c r="AB36" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="5">
         <v>4500992800</v>
       </c>
-      <c r="AD36" t="s">
+      <c r="AE36" t="s">
         <v>70</v>
       </c>
-      <c r="AE36">
-        <v>0</v>
-      </c>
-      <c r="AG36" t="s">
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AH36" t="s">
         <v>304</v>
       </c>
-      <c r="AI36" s="2">
+      <c r="AJ36" s="2">
         <v>42309</v>
       </c>
-      <c r="AJ36" s="2">
+      <c r="AK36" s="2">
         <v>44135</v>
       </c>
-      <c r="AK36" t="s">
+      <c r="AL36" t="s">
         <v>71</v>
       </c>
-      <c r="AL36" t="s">
-        <v>72</v>
-      </c>
       <c r="AM36" t="s">
         <v>72</v>
       </c>
-      <c r="AN36" s="8"/>
-      <c r="AO36" s="1">
+      <c r="AN36" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO36" s="8"/>
+      <c r="AP36" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP36" t="s">
+      <c r="AQ36" t="s">
         <v>281</v>
       </c>
-      <c r="AQ36" t="s">
+      <c r="AR36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:44">
       <c r="A37" t="s">
         <v>309</v>
       </c>
@@ -6230,47 +5757,50 @@
         <v>3150000</v>
       </c>
       <c r="AB37" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="5">
         <v>4500992802</v>
       </c>
-      <c r="AD37" t="s">
+      <c r="AE37" t="s">
         <v>70</v>
       </c>
-      <c r="AE37">
-        <v>0</v>
-      </c>
-      <c r="AG37" t="s">
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AH37" t="s">
         <v>310</v>
       </c>
-      <c r="AI37" s="2">
+      <c r="AJ37" s="2">
         <v>42323</v>
       </c>
-      <c r="AJ37" s="2">
+      <c r="AK37" s="2">
         <v>44149</v>
       </c>
-      <c r="AK37" t="s">
+      <c r="AL37" t="s">
         <v>71</v>
       </c>
-      <c r="AL37" t="s">
-        <v>72</v>
-      </c>
       <c r="AM37" t="s">
         <v>72</v>
       </c>
-      <c r="AN37" s="8"/>
-      <c r="AO37" s="1">
+      <c r="AN37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO37" s="8"/>
+      <c r="AP37" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP37" t="s">
+      <c r="AQ37" t="s">
         <v>281</v>
       </c>
-      <c r="AQ37" t="s">
+      <c r="AR37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:44">
       <c r="A38" t="s">
         <v>314</v>
       </c>
@@ -6341,47 +5871,50 @@
         <v>3150000</v>
       </c>
       <c r="AB38" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="5">
         <v>4500992802</v>
       </c>
-      <c r="AD38" t="s">
+      <c r="AE38" t="s">
         <v>120</v>
       </c>
-      <c r="AE38">
-        <v>0</v>
-      </c>
-      <c r="AG38" t="s">
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AH38" t="s">
         <v>315</v>
       </c>
-      <c r="AI38" s="2">
+      <c r="AJ38" s="2">
         <v>42323</v>
       </c>
-      <c r="AJ38" s="2">
+      <c r="AK38" s="2">
         <v>44149</v>
       </c>
-      <c r="AK38" t="s">
+      <c r="AL38" t="s">
         <v>71</v>
       </c>
-      <c r="AL38" t="s">
-        <v>72</v>
-      </c>
       <c r="AM38" t="s">
         <v>72</v>
       </c>
-      <c r="AN38" s="8"/>
-      <c r="AO38" s="1">
+      <c r="AN38" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO38" s="8"/>
+      <c r="AP38" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP38" t="s">
+      <c r="AQ38" t="s">
         <v>281</v>
       </c>
-      <c r="AQ38" t="s">
+      <c r="AR38" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:44">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -6452,47 +5985,50 @@
         <v>3150000</v>
       </c>
       <c r="AB39" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="5">
         <v>4500992780</v>
       </c>
-      <c r="AD39" t="s">
+      <c r="AE39" t="s">
         <v>70</v>
       </c>
-      <c r="AE39">
-        <v>0</v>
-      </c>
-      <c r="AG39" t="s">
+      <c r="AF39">
+        <v>0</v>
+      </c>
+      <c r="AH39" t="s">
         <v>321</v>
       </c>
-      <c r="AI39" s="2">
+      <c r="AJ39" s="2">
         <v>42323</v>
       </c>
-      <c r="AJ39" s="2">
+      <c r="AK39" s="2">
         <v>44149</v>
       </c>
-      <c r="AK39" t="s">
+      <c r="AL39" t="s">
         <v>71</v>
       </c>
-      <c r="AL39" t="s">
-        <v>72</v>
-      </c>
       <c r="AM39" t="s">
         <v>72</v>
       </c>
-      <c r="AN39" s="8"/>
-      <c r="AO39" s="1">
+      <c r="AN39" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO39" s="8"/>
+      <c r="AP39" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP39" t="s">
+      <c r="AQ39" t="s">
         <v>281</v>
       </c>
-      <c r="AQ39" t="s">
+      <c r="AR39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:43">
+    <row r="40" spans="1:44">
       <c r="A40" t="s">
         <v>326</v>
       </c>
@@ -6563,47 +6099,50 @@
         <v>3150000</v>
       </c>
       <c r="AB40" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="5">
         <v>4500992780</v>
       </c>
-      <c r="AD40" t="s">
+      <c r="AE40" t="s">
         <v>120</v>
       </c>
-      <c r="AE40">
-        <v>0</v>
-      </c>
-      <c r="AG40" t="s">
+      <c r="AF40">
+        <v>0</v>
+      </c>
+      <c r="AH40" t="s">
         <v>327</v>
       </c>
-      <c r="AI40" s="2">
+      <c r="AJ40" s="2">
         <v>42323</v>
       </c>
-      <c r="AJ40" s="2">
+      <c r="AK40" s="2">
         <v>44149</v>
       </c>
-      <c r="AK40" t="s">
+      <c r="AL40" t="s">
         <v>71</v>
       </c>
-      <c r="AL40" t="s">
-        <v>72</v>
-      </c>
       <c r="AM40" t="s">
         <v>72</v>
       </c>
-      <c r="AN40" s="8"/>
-      <c r="AO40" s="1">
+      <c r="AN40" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO40" s="8"/>
+      <c r="AP40" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP40" t="s">
+      <c r="AQ40" t="s">
         <v>281</v>
       </c>
-      <c r="AQ40" t="s">
+      <c r="AR40" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:43">
+    <row r="41" spans="1:44">
       <c r="A41" t="s">
         <v>331</v>
       </c>
@@ -6674,47 +6213,50 @@
         <v>3150000</v>
       </c>
       <c r="AB41" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="5">
         <v>4500992780</v>
       </c>
-      <c r="AD41" t="s">
+      <c r="AE41" t="s">
         <v>250</v>
       </c>
-      <c r="AE41">
-        <v>0</v>
-      </c>
-      <c r="AG41" t="s">
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AH41" t="s">
         <v>332</v>
       </c>
-      <c r="AI41" s="2">
+      <c r="AJ41" s="2">
         <v>42323</v>
       </c>
-      <c r="AJ41" s="2">
+      <c r="AK41" s="2">
         <v>44149</v>
       </c>
-      <c r="AK41" t="s">
+      <c r="AL41" t="s">
         <v>71</v>
       </c>
-      <c r="AL41" t="s">
-        <v>72</v>
-      </c>
       <c r="AM41" t="s">
         <v>72</v>
       </c>
-      <c r="AN41" s="8"/>
-      <c r="AO41" s="1">
+      <c r="AN41" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO41" s="8"/>
+      <c r="AP41" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP41" t="s">
+      <c r="AQ41" t="s">
         <v>281</v>
       </c>
-      <c r="AQ41" t="s">
+      <c r="AR41" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:42">
+    <row r="42" spans="1:44">
       <c r="A42" t="s">
         <v>336</v>
       </c>
@@ -6785,41 +6327,44 @@
         <v>7010000</v>
       </c>
       <c r="AB42" s="1">
+        <v>7010000</v>
+      </c>
+      <c r="AC42" s="1">
         <v>701000</v>
       </c>
-      <c r="AC42" s="5">
+      <c r="AD42" s="5">
         <v>4500985023</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>70</v>
       </c>
-      <c r="AE42">
+      <c r="AF42">
         <v>1</v>
       </c>
-      <c r="AI42" s="2">
+      <c r="AJ42" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ42" s="2">
+      <c r="AK42" s="2">
         <v>44043</v>
       </c>
-      <c r="AK42" t="s">
+      <c r="AL42" t="s">
         <v>71</v>
       </c>
-      <c r="AL42" t="s">
-        <v>72</v>
-      </c>
       <c r="AM42" t="s">
         <v>72</v>
       </c>
-      <c r="AN42" s="8"/>
-      <c r="AO42" s="1">
+      <c r="AN42" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO42" s="8"/>
+      <c r="AP42" s="1">
         <v>7711000</v>
       </c>
-      <c r="AP42" t="s">
+      <c r="AQ42" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:44">
       <c r="A43" t="s">
         <v>345</v>
       </c>
@@ -6890,47 +6435,50 @@
         <v>2890000</v>
       </c>
       <c r="AB43" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="5">
         <v>4500705483</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AE43" t="s">
         <v>120</v>
       </c>
-      <c r="AE43">
-        <v>0</v>
-      </c>
-      <c r="AG43" t="s">
+      <c r="AF43">
+        <v>0</v>
+      </c>
+      <c r="AH43" t="s">
         <v>346</v>
       </c>
-      <c r="AI43" s="2">
+      <c r="AJ43" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ43" s="2">
+      <c r="AK43" s="2">
         <v>43465</v>
       </c>
-      <c r="AK43" t="s">
+      <c r="AL43" t="s">
         <v>71</v>
       </c>
-      <c r="AL43" t="s">
-        <v>72</v>
-      </c>
       <c r="AM43" t="s">
         <v>72</v>
       </c>
-      <c r="AN43" s="8"/>
-      <c r="AO43" s="1">
+      <c r="AN43" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO43" s="8"/>
+      <c r="AP43" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP43" t="s">
+      <c r="AQ43" t="s">
         <v>95</v>
       </c>
-      <c r="AQ43" t="s">
+      <c r="AR43" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:44">
       <c r="A44" t="s">
         <v>350</v>
       </c>
@@ -7001,47 +6549,50 @@
         <v>3150000</v>
       </c>
       <c r="AB44" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="5">
         <v>4500990107</v>
       </c>
-      <c r="AD44" t="s">
+      <c r="AE44" t="s">
         <v>70</v>
       </c>
-      <c r="AE44">
-        <v>0</v>
-      </c>
-      <c r="AG44" t="s">
+      <c r="AF44">
+        <v>0</v>
+      </c>
+      <c r="AH44" t="s">
         <v>351</v>
       </c>
-      <c r="AI44" s="2">
+      <c r="AJ44" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ44" s="2">
+      <c r="AK44" s="2">
         <v>44043</v>
       </c>
-      <c r="AK44" t="s">
+      <c r="AL44" t="s">
         <v>71</v>
       </c>
-      <c r="AL44" t="s">
-        <v>72</v>
-      </c>
       <c r="AM44" t="s">
         <v>72</v>
       </c>
-      <c r="AN44" s="8"/>
-      <c r="AO44" s="1">
+      <c r="AN44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO44" s="8"/>
+      <c r="AP44" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP44" t="s">
+      <c r="AQ44" t="s">
         <v>95</v>
       </c>
-      <c r="AQ44" t="s">
+      <c r="AR44" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:43">
+    <row r="45" spans="1:44">
       <c r="A45" t="s">
         <v>355</v>
       </c>
@@ -7112,47 +6663,50 @@
         <v>3150000</v>
       </c>
       <c r="AB45" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="5">
         <v>4500990135</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AE45" t="s">
         <v>70</v>
       </c>
-      <c r="AE45">
-        <v>0</v>
-      </c>
-      <c r="AG45" t="s">
+      <c r="AF45">
+        <v>0</v>
+      </c>
+      <c r="AH45" t="s">
         <v>356</v>
       </c>
-      <c r="AI45" s="2">
+      <c r="AJ45" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ45" s="2">
+      <c r="AK45" s="2">
         <v>44043</v>
       </c>
-      <c r="AK45" t="s">
+      <c r="AL45" t="s">
         <v>71</v>
       </c>
-      <c r="AL45" t="s">
-        <v>72</v>
-      </c>
       <c r="AM45" t="s">
         <v>72</v>
       </c>
-      <c r="AN45" s="8"/>
-      <c r="AO45" s="1">
+      <c r="AN45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO45" s="8"/>
+      <c r="AP45" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP45" t="s">
+      <c r="AQ45" t="s">
         <v>95</v>
       </c>
-      <c r="AQ45" t="s">
+      <c r="AR45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:44">
       <c r="A46" t="s">
         <v>360</v>
       </c>
@@ -7223,47 +6777,50 @@
         <v>3150000</v>
       </c>
       <c r="AB46" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="5">
         <v>4500990135</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AE46" t="s">
         <v>120</v>
       </c>
-      <c r="AE46">
-        <v>0</v>
-      </c>
-      <c r="AG46" t="s">
+      <c r="AF46">
+        <v>0</v>
+      </c>
+      <c r="AH46" t="s">
         <v>361</v>
       </c>
-      <c r="AI46" s="2">
+      <c r="AJ46" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ46" s="2">
+      <c r="AK46" s="2">
         <v>44043</v>
       </c>
-      <c r="AK46" t="s">
+      <c r="AL46" t="s">
         <v>71</v>
       </c>
-      <c r="AL46" t="s">
-        <v>72</v>
-      </c>
       <c r="AM46" t="s">
         <v>72</v>
       </c>
-      <c r="AN46" s="8"/>
-      <c r="AO46" s="1">
+      <c r="AN46" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO46" s="8"/>
+      <c r="AP46" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP46" t="s">
+      <c r="AQ46" t="s">
         <v>95</v>
       </c>
-      <c r="AQ46" t="s">
+      <c r="AR46" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:44">
       <c r="A47" t="s">
         <v>365</v>
       </c>
@@ -7334,47 +6891,50 @@
         <v>3150000</v>
       </c>
       <c r="AB47" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="5">
         <v>4500990135</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AE47" t="s">
         <v>250</v>
       </c>
-      <c r="AE47">
-        <v>0</v>
-      </c>
-      <c r="AG47" t="s">
+      <c r="AF47">
+        <v>0</v>
+      </c>
+      <c r="AH47" t="s">
         <v>366</v>
       </c>
-      <c r="AI47" s="2">
+      <c r="AJ47" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ47" s="2">
+      <c r="AK47" s="2">
         <v>44043</v>
       </c>
-      <c r="AK47" t="s">
+      <c r="AL47" t="s">
         <v>71</v>
       </c>
-      <c r="AL47" t="s">
-        <v>72</v>
-      </c>
       <c r="AM47" t="s">
         <v>72</v>
       </c>
-      <c r="AN47" s="8"/>
-      <c r="AO47" s="1">
+      <c r="AN47" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO47" s="8"/>
+      <c r="AP47" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP47" t="s">
+      <c r="AQ47" t="s">
         <v>95</v>
       </c>
-      <c r="AQ47" t="s">
+      <c r="AR47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:44">
       <c r="A48" t="s">
         <v>370</v>
       </c>
@@ -7445,47 +7005,50 @@
         <v>3150000</v>
       </c>
       <c r="AB48" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="5">
+        <v>3150000</v>
+      </c>
+      <c r="AC48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="5">
         <v>4501000803</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AE48" t="s">
         <v>70</v>
       </c>
-      <c r="AE48">
-        <v>0</v>
-      </c>
-      <c r="AG48" t="s">
+      <c r="AF48">
+        <v>0</v>
+      </c>
+      <c r="AH48" t="s">
         <v>371</v>
       </c>
-      <c r="AI48" s="2">
+      <c r="AJ48" s="2">
         <v>42217</v>
       </c>
-      <c r="AJ48" s="2">
+      <c r="AK48" s="2">
         <v>44043</v>
       </c>
-      <c r="AK48" t="s">
+      <c r="AL48" t="s">
         <v>71</v>
       </c>
-      <c r="AL48" t="s">
-        <v>72</v>
-      </c>
       <c r="AM48" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN48" t="s">
         <v>375</v>
       </c>
-      <c r="AN48" s="8"/>
-      <c r="AO48" s="1">
+      <c r="AO48" s="8"/>
+      <c r="AP48" s="1">
         <v>3150000</v>
       </c>
-      <c r="AP48" t="s">
+      <c r="AQ48" t="s">
         <v>281</v>
       </c>
-      <c r="AQ48" t="s">
+      <c r="AR48" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:43">
+    <row r="49" spans="1:44">
       <c r="A49" t="s">
         <v>376</v>
       </c>
@@ -7556,44 +7119,47 @@
         <v>5672100</v>
       </c>
       <c r="AB49" s="1">
+        <v>5672100</v>
+      </c>
+      <c r="AC49" s="1">
         <v>567210</v>
       </c>
-      <c r="AC49" s="5">
+      <c r="AD49" s="5">
         <v>4500751711</v>
       </c>
-      <c r="AD49" t="s">
+      <c r="AE49" t="s">
         <v>176</v>
       </c>
-      <c r="AE49">
+      <c r="AF49">
         <v>1</v>
       </c>
-      <c r="AI49" s="2">
+      <c r="AJ49" s="2">
         <v>41532</v>
       </c>
-      <c r="AJ49" s="2">
+      <c r="AK49" s="2">
         <v>43357</v>
       </c>
-      <c r="AK49" t="s">
+      <c r="AL49" t="s">
         <v>71</v>
       </c>
-      <c r="AL49" t="s">
-        <v>72</v>
-      </c>
       <c r="AM49" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN49" t="s">
         <v>383</v>
       </c>
-      <c r="AN49" s="8"/>
-      <c r="AO49" s="1">
+      <c r="AO49" s="8"/>
+      <c r="AP49" s="1">
         <v>6239310</v>
       </c>
-      <c r="AP49" t="s">
+      <c r="AQ49" t="s">
         <v>281</v>
       </c>
-      <c r="AQ49" t="s">
+      <c r="AR49" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:43">
+    <row r="50" spans="1:44">
       <c r="A50" t="s">
         <v>384</v>
       </c>
@@ -7664,47 +7230,50 @@
         <v>2890000</v>
       </c>
       <c r="AB50" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC50" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="5">
         <v>4500705640</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AE50" t="s">
         <v>120</v>
       </c>
-      <c r="AE50">
-        <v>0</v>
-      </c>
-      <c r="AG50" t="s">
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AH50" t="s">
         <v>385</v>
       </c>
-      <c r="AI50" s="2">
+      <c r="AJ50" s="2">
         <v>41640</v>
       </c>
-      <c r="AJ50" s="2">
+      <c r="AK50" s="2">
         <v>43465</v>
       </c>
-      <c r="AK50" t="s">
+      <c r="AL50" t="s">
         <v>71</v>
       </c>
-      <c r="AL50" t="s">
-        <v>72</v>
-      </c>
       <c r="AM50" t="s">
         <v>72</v>
       </c>
-      <c r="AN50" s="8"/>
-      <c r="AO50" s="1">
+      <c r="AN50" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO50" s="8"/>
+      <c r="AP50" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP50" t="s">
+      <c r="AQ50" t="s">
         <v>95</v>
       </c>
-      <c r="AQ50" t="s">
+      <c r="AR50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:43">
+    <row r="51" spans="1:44">
       <c r="A51" t="s">
         <v>389</v>
       </c>
@@ -7775,47 +7344,50 @@
         <v>2890000</v>
       </c>
       <c r="AB51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC51" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="5">
         <v>4500663217</v>
       </c>
-      <c r="AD51" t="s">
+      <c r="AE51" t="s">
         <v>70</v>
       </c>
-      <c r="AE51">
-        <v>0</v>
-      </c>
-      <c r="AG51" t="s">
+      <c r="AF51">
+        <v>0</v>
+      </c>
+      <c r="AH51" t="s">
         <v>390</v>
       </c>
-      <c r="AI51" s="2">
+      <c r="AJ51" s="2">
         <v>41487</v>
       </c>
-      <c r="AJ51" s="2">
+      <c r="AK51" s="2">
         <v>43312</v>
       </c>
-      <c r="AK51" t="s">
+      <c r="AL51" t="s">
         <v>71</v>
       </c>
-      <c r="AL51" t="s">
-        <v>72</v>
-      </c>
       <c r="AM51" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN51" t="s">
         <v>394</v>
       </c>
-      <c r="AN51" s="8"/>
-      <c r="AO51" s="1">
+      <c r="AO51" s="8"/>
+      <c r="AP51" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP51" t="s">
+      <c r="AQ51" t="s">
         <v>95</v>
       </c>
-      <c r="AQ51" t="s">
+      <c r="AR51" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:43">
+    <row r="52" spans="1:44">
       <c r="A52" t="s">
         <v>395</v>
       </c>
@@ -7886,51 +7458,53 @@
         <v>2890000</v>
       </c>
       <c r="AB52" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC52" s="5">
+        <v>2890000</v>
+      </c>
+      <c r="AC52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="5">
         <v>4500677457</v>
       </c>
-      <c r="AD52" t="s">
+      <c r="AE52" t="s">
         <v>70</v>
       </c>
-      <c r="AE52">
-        <v>0</v>
-      </c>
-      <c r="AG52" t="s">
+      <c r="AF52">
+        <v>0</v>
+      </c>
+      <c r="AH52" t="s">
         <v>396</v>
       </c>
-      <c r="AI52" s="2">
+      <c r="AJ52" s="2">
         <v>41487</v>
       </c>
-      <c r="AJ52" s="2">
+      <c r="AK52" s="2">
         <v>43312</v>
       </c>
-      <c r="AK52" t="s">
+      <c r="AL52" t="s">
         <v>71</v>
       </c>
-      <c r="AL52" t="s">
-        <v>72</v>
-      </c>
       <c r="AM52" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN52" t="s">
         <v>400</v>
       </c>
-      <c r="AN52" s="8"/>
-      <c r="AO52" s="1">
+      <c r="AO52" s="8"/>
+      <c r="AP52" s="1">
         <v>2890000</v>
       </c>
-      <c r="AP52" t="s">
+      <c r="AQ52" t="s">
         <v>281</v>
       </c>
-      <c r="AQ52" t="s">
+      <c r="AR52" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AV52"/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <autoFilter ref="A3:AW52"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix master location mapping
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/masterFleet.xlsx
+++ b/FMS.Website/files_upload/masterFleet.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AW$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AV$53</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -89,34 +89,12 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-data dari master data price list</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Gani, Ida:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
 Jika Restition = No, maka VAT = 10%* Monthly HMS Installment
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="AI3" authorId="0" shapeId="0">
+    <comment ref="AH3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ3" authorId="0" shapeId="0">
+    <comment ref="AP3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR3" authorId="0" shapeId="0">
+    <comment ref="AQ3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>MASTER DATA FLEET</t>
   </si>
@@ -331,9 +309,6 @@
   </si>
   <si>
     <t>Modified Date</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -697,13 +672,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW53"/>
+  <dimension ref="A1:AV53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -715,27 +690,28 @@
     <col min="17" max="17" width="14.42578125" customWidth="1"/>
     <col min="18" max="20" width="19.140625" customWidth="1"/>
     <col min="23" max="25" width="8.7109375" customWidth="1"/>
-    <col min="27" max="28" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="32" width="8.7109375" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" customWidth="1"/>
-    <col min="35" max="37" width="9.85546875" style="2" customWidth="1"/>
-    <col min="38" max="38" width="18" customWidth="1"/>
-    <col min="40" max="41" width="8.7109375" customWidth="1"/>
-    <col min="42" max="42" width="19" style="1" customWidth="1"/>
-    <col min="43" max="43" width="14.5703125" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" customWidth="1"/>
+    <col min="27" max="27" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11" customWidth="1"/>
+    <col min="30" max="31" width="8.7109375" customWidth="1"/>
+    <col min="32" max="32" width="11.7109375" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" customWidth="1"/>
+    <col min="34" max="36" width="9.85546875" style="2" customWidth="1"/>
+    <col min="37" max="37" width="18" customWidth="1"/>
+    <col min="39" max="40" width="8.7109375" customWidth="1"/>
+    <col min="41" max="41" width="19" style="1" customWidth="1"/>
+    <col min="42" max="42" width="14.5703125" customWidth="1"/>
+    <col min="43" max="43" width="13.5703125" customWidth="1"/>
+    <col min="48" max="48" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:48">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="15" customHeight="1"/>
-    <row r="3" spans="1:49">
+    <row r="2" spans="1:48" ht="15" customHeight="1"/>
+    <row r="3" spans="1:48">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -818,73 +794,70 @@
         <v>27</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AC3" t="s">
+        <v>29</v>
+      </c>
       <c r="AD3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE3" t="s">
         <v>30</v>
       </c>
+      <c r="AE3" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="AF3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="AI3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="AJ3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AK3" t="s">
         <v>37</v>
       </c>
+      <c r="AL3" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AM3" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AN3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AO3" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="AP3" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="AQ3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR3" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AR3" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="AS3" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AU3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AV3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49">
+    </row>
+    <row r="4" spans="1:48">
       <c r="H4" s="4"/>
       <c r="M4" s="4"/>
       <c r="P4" s="4"/>
@@ -895,23 +868,23 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="Z4" s="4"/>
+      <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AL4" s="7"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="10"/>
       <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
+      <c r="AR4" s="4"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
       <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-    </row>
-    <row r="5" spans="1:49">
+    </row>
+    <row r="5" spans="1:48">
       <c r="H5" s="4"/>
       <c r="M5" s="4"/>
       <c r="P5" s="4"/>
@@ -922,23 +895,23 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="Z5" s="4"/>
+      <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AL5" s="7"/>
       <c r="AM5" s="7"/>
       <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="10"/>
       <c r="AQ5" s="10"/>
-      <c r="AR5" s="10"/>
+      <c r="AR5" s="4"/>
       <c r="AS5" s="4"/>
       <c r="AT5" s="4"/>
       <c r="AU5" s="4"/>
       <c r="AV5" s="4"/>
-      <c r="AW5" s="4"/>
-    </row>
-    <row r="6" spans="1:49">
+    </row>
+    <row r="6" spans="1:48">
       <c r="H6" s="4"/>
       <c r="M6" s="4"/>
       <c r="P6" s="4"/>
@@ -949,23 +922,23 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="Z6" s="4"/>
+      <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="10"/>
       <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
+      <c r="AR6" s="4"/>
       <c r="AS6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
-      <c r="AW6" s="4"/>
-    </row>
-    <row r="7" spans="1:49">
+    </row>
+    <row r="7" spans="1:48">
       <c r="H7" s="4"/>
       <c r="M7" s="4"/>
       <c r="P7" s="4"/>
@@ -976,23 +949,23 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="Z7" s="4"/>
+      <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="10"/>
       <c r="AQ7" s="10"/>
-      <c r="AR7" s="10"/>
+      <c r="AR7" s="4"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
       <c r="AV7" s="4"/>
-      <c r="AW7" s="4"/>
-    </row>
-    <row r="8" spans="1:49">
+    </row>
+    <row r="8" spans="1:48">
       <c r="H8" s="4"/>
       <c r="M8" s="4"/>
       <c r="P8" s="4"/>
@@ -1003,23 +976,23 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="Z8" s="4"/>
+      <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="10"/>
       <c r="AQ8" s="10"/>
-      <c r="AR8" s="10"/>
+      <c r="AR8" s="4"/>
       <c r="AS8" s="4"/>
       <c r="AT8" s="4"/>
       <c r="AU8" s="4"/>
       <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-    </row>
-    <row r="9" spans="1:49">
+    </row>
+    <row r="9" spans="1:48">
       <c r="H9" s="4"/>
       <c r="M9" s="4"/>
       <c r="P9" s="4"/>
@@ -1030,23 +1003,23 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="Z9" s="4"/>
+      <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AL9" s="7"/>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="10"/>
       <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
+      <c r="AR9" s="4"/>
       <c r="AS9" s="4"/>
       <c r="AT9" s="4"/>
       <c r="AU9" s="4"/>
       <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-    </row>
-    <row r="10" spans="1:49">
+    </row>
+    <row r="10" spans="1:48">
       <c r="H10" s="4"/>
       <c r="M10" s="4"/>
       <c r="P10" s="4"/>
@@ -1057,23 +1030,23 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="Z10" s="4"/>
+      <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AL10" s="7"/>
       <c r="AM10" s="7"/>
       <c r="AN10" s="7"/>
-      <c r="AO10" s="7"/>
-      <c r="AP10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="10"/>
       <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
+      <c r="AR10" s="4"/>
       <c r="AS10" s="4"/>
       <c r="AT10" s="4"/>
       <c r="AU10" s="4"/>
       <c r="AV10" s="4"/>
-      <c r="AW10" s="4"/>
-    </row>
-    <row r="11" spans="1:49">
+    </row>
+    <row r="11" spans="1:48">
       <c r="H11" s="4"/>
       <c r="M11" s="4"/>
       <c r="P11" s="4"/>
@@ -1084,23 +1057,23 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="Z11" s="4"/>
+      <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AL11" s="7"/>
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="10"/>
       <c r="AQ11" s="10"/>
-      <c r="AR11" s="10"/>
+      <c r="AR11" s="4"/>
       <c r="AS11" s="4"/>
       <c r="AT11" s="4"/>
       <c r="AU11" s="4"/>
       <c r="AV11" s="4"/>
-      <c r="AW11" s="4"/>
-    </row>
-    <row r="12" spans="1:49">
+    </row>
+    <row r="12" spans="1:48">
       <c r="H12" s="4"/>
       <c r="M12" s="4"/>
       <c r="P12" s="4"/>
@@ -1111,23 +1084,23 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="Z12" s="4"/>
+      <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AL12" s="7"/>
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="10"/>
       <c r="AQ12" s="10"/>
-      <c r="AR12" s="10"/>
+      <c r="AR12" s="4"/>
       <c r="AS12" s="4"/>
       <c r="AT12" s="4"/>
       <c r="AU12" s="4"/>
       <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-    </row>
-    <row r="13" spans="1:49">
+    </row>
+    <row r="13" spans="1:48">
       <c r="H13" s="4"/>
       <c r="M13" s="4"/>
       <c r="P13" s="4"/>
@@ -1138,23 +1111,23 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="Z13" s="4"/>
+      <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AL13" s="7"/>
       <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="10"/>
       <c r="AQ13" s="10"/>
-      <c r="AR13" s="10"/>
+      <c r="AR13" s="4"/>
       <c r="AS13" s="4"/>
       <c r="AT13" s="4"/>
       <c r="AU13" s="4"/>
       <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-    </row>
-    <row r="14" spans="1:49">
+    </row>
+    <row r="14" spans="1:48">
       <c r="H14" s="4"/>
       <c r="M14" s="4"/>
       <c r="P14" s="4"/>
@@ -1165,23 +1138,23 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="Z14" s="4"/>
+      <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AL14" s="7"/>
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="9"/>
+      <c r="AO14" s="9"/>
+      <c r="AP14" s="10"/>
       <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
+      <c r="AR14" s="4"/>
       <c r="AS14" s="4"/>
       <c r="AT14" s="4"/>
       <c r="AU14" s="4"/>
       <c r="AV14" s="4"/>
-      <c r="AW14" s="4"/>
-    </row>
-    <row r="15" spans="1:49">
+    </row>
+    <row r="15" spans="1:48">
       <c r="H15" s="4"/>
       <c r="M15" s="4"/>
       <c r="P15" s="4"/>
@@ -1192,23 +1165,23 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="Z15" s="4"/>
+      <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AL15" s="7"/>
       <c r="AM15" s="7"/>
       <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="9"/>
+      <c r="AO15" s="9"/>
+      <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
-      <c r="AR15" s="10"/>
+      <c r="AR15" s="4"/>
       <c r="AS15" s="4"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
-      <c r="AW15" s="4"/>
-    </row>
-    <row r="16" spans="1:49">
+    </row>
+    <row r="16" spans="1:48">
       <c r="H16" s="4"/>
       <c r="M16" s="4"/>
       <c r="P16" s="4"/>
@@ -1219,23 +1192,23 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="Z16" s="4"/>
+      <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
-      <c r="AH16" s="4"/>
-      <c r="AI16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AL16" s="7"/>
       <c r="AM16" s="7"/>
       <c r="AN16" s="7"/>
-      <c r="AO16" s="7"/>
-      <c r="AP16" s="9"/>
+      <c r="AO16" s="9"/>
+      <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
-      <c r="AR16" s="10"/>
+      <c r="AR16" s="4"/>
       <c r="AS16" s="4"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
-      <c r="AW16" s="4"/>
-    </row>
-    <row r="17" spans="8:49">
+    </row>
+    <row r="17" spans="8:48">
       <c r="H17" s="4"/>
       <c r="M17" s="4"/>
       <c r="P17" s="4"/>
@@ -1246,23 +1219,23 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
       <c r="Z17" s="4"/>
+      <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AL17" s="7"/>
       <c r="AM17" s="7"/>
       <c r="AN17" s="7"/>
-      <c r="AO17" s="7"/>
-      <c r="AP17" s="9"/>
+      <c r="AO17" s="9"/>
+      <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
-      <c r="AR17" s="10"/>
+      <c r="AR17" s="4"/>
       <c r="AS17" s="4"/>
       <c r="AT17" s="4"/>
       <c r="AU17" s="4"/>
       <c r="AV17" s="4"/>
-      <c r="AW17" s="4"/>
-    </row>
-    <row r="18" spans="8:49">
+    </row>
+    <row r="18" spans="8:48">
       <c r="H18" s="4"/>
       <c r="M18" s="4"/>
       <c r="P18" s="4"/>
@@ -1273,23 +1246,23 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="Z18" s="4"/>
+      <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AL18" s="7"/>
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
-      <c r="AO18" s="7"/>
-      <c r="AP18" s="9"/>
+      <c r="AO18" s="9"/>
+      <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
-      <c r="AR18" s="10"/>
+      <c r="AR18" s="4"/>
       <c r="AS18" s="4"/>
       <c r="AT18" s="4"/>
       <c r="AU18" s="4"/>
       <c r="AV18" s="4"/>
-      <c r="AW18" s="4"/>
-    </row>
-    <row r="19" spans="8:49">
+    </row>
+    <row r="19" spans="8:48">
       <c r="H19" s="4"/>
       <c r="M19" s="4"/>
       <c r="P19" s="4"/>
@@ -1300,160 +1273,160 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="Z19" s="4"/>
+      <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AL19" s="7"/>
       <c r="AM19" s="7"/>
       <c r="AN19" s="7"/>
-      <c r="AO19" s="7"/>
-      <c r="AP19" s="9"/>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="10"/>
       <c r="AQ19" s="10"/>
-      <c r="AR19" s="10"/>
+      <c r="AR19" s="4"/>
       <c r="AS19" s="4"/>
       <c r="AT19" s="4"/>
       <c r="AU19" s="4"/>
       <c r="AV19" s="4"/>
-      <c r="AW19" s="4"/>
-    </row>
-    <row r="20" spans="8:49">
-      <c r="AD20" s="5"/>
-      <c r="AO20" s="8"/>
-    </row>
-    <row r="21" spans="8:49">
-      <c r="AD21" s="5"/>
-      <c r="AO21" s="8"/>
-    </row>
-    <row r="22" spans="8:49">
-      <c r="AD22" s="5"/>
-      <c r="AO22" s="8"/>
-    </row>
-    <row r="23" spans="8:49">
-      <c r="AD23" s="5"/>
-      <c r="AO23" s="8"/>
-    </row>
-    <row r="24" spans="8:49">
-      <c r="AD24" s="5"/>
-      <c r="AO24" s="8"/>
-    </row>
-    <row r="25" spans="8:49">
-      <c r="AD25" s="5"/>
-      <c r="AO25" s="8"/>
-    </row>
-    <row r="26" spans="8:49">
-      <c r="AD26" s="5"/>
-      <c r="AO26" s="8"/>
-    </row>
-    <row r="27" spans="8:49">
-      <c r="AD27" s="5"/>
-      <c r="AO27" s="8"/>
-    </row>
-    <row r="28" spans="8:49">
-      <c r="AD28" s="5"/>
-      <c r="AO28" s="8"/>
-    </row>
-    <row r="29" spans="8:49">
-      <c r="AD29" s="5"/>
-      <c r="AO29" s="8"/>
-    </row>
-    <row r="30" spans="8:49">
-      <c r="AD30" s="5"/>
-      <c r="AO30" s="8"/>
-    </row>
-    <row r="31" spans="8:49">
-      <c r="AD31" s="5"/>
-      <c r="AO31" s="8"/>
-    </row>
-    <row r="32" spans="8:49">
-      <c r="AD32" s="5"/>
-      <c r="AO32" s="8"/>
-    </row>
-    <row r="33" spans="30:41">
-      <c r="AD33" s="5"/>
-      <c r="AO33" s="8"/>
-    </row>
-    <row r="34" spans="30:41">
-      <c r="AD34" s="5"/>
-      <c r="AO34" s="8"/>
-    </row>
-    <row r="35" spans="30:41">
-      <c r="AD35" s="5"/>
-      <c r="AO35" s="8"/>
-    </row>
-    <row r="36" spans="30:41">
-      <c r="AD36" s="5"/>
-      <c r="AO36" s="8"/>
-    </row>
-    <row r="37" spans="30:41">
-      <c r="AD37" s="5"/>
-      <c r="AO37" s="8"/>
-    </row>
-    <row r="38" spans="30:41">
-      <c r="AD38" s="5"/>
-      <c r="AO38" s="8"/>
-    </row>
-    <row r="39" spans="30:41">
-      <c r="AD39" s="5"/>
-      <c r="AO39" s="8"/>
-    </row>
-    <row r="40" spans="30:41">
-      <c r="AD40" s="5"/>
-      <c r="AO40" s="8"/>
-    </row>
-    <row r="41" spans="30:41">
-      <c r="AD41" s="5"/>
-      <c r="AO41" s="8"/>
-    </row>
-    <row r="42" spans="30:41">
-      <c r="AD42" s="5"/>
-      <c r="AO42" s="8"/>
-    </row>
-    <row r="43" spans="30:41">
-      <c r="AD43" s="5"/>
-      <c r="AO43" s="8"/>
-    </row>
-    <row r="44" spans="30:41">
-      <c r="AD44" s="5"/>
-      <c r="AO44" s="8"/>
-    </row>
-    <row r="45" spans="30:41">
-      <c r="AD45" s="5"/>
-      <c r="AO45" s="8"/>
-    </row>
-    <row r="46" spans="30:41">
-      <c r="AD46" s="5"/>
-      <c r="AO46" s="8"/>
-    </row>
-    <row r="47" spans="30:41">
-      <c r="AD47" s="5"/>
-      <c r="AO47" s="8"/>
-    </row>
-    <row r="48" spans="30:41">
-      <c r="AD48" s="5"/>
-      <c r="AO48" s="8"/>
-    </row>
-    <row r="49" spans="30:41">
-      <c r="AD49" s="5"/>
-      <c r="AO49" s="8"/>
-    </row>
-    <row r="50" spans="30:41">
-      <c r="AD50" s="5"/>
-      <c r="AO50" s="8"/>
-    </row>
-    <row r="51" spans="30:41">
-      <c r="AD51" s="5"/>
-      <c r="AO51" s="8"/>
-    </row>
-    <row r="52" spans="30:41">
-      <c r="AD52" s="5"/>
-      <c r="AO52" s="8"/>
-    </row>
-    <row r="53" spans="30:41">
-      <c r="AD53" s="5"/>
-      <c r="AO53" s="8"/>
+    </row>
+    <row r="20" spans="8:48">
+      <c r="AC20" s="5"/>
+      <c r="AN20" s="8"/>
+    </row>
+    <row r="21" spans="8:48">
+      <c r="AC21" s="5"/>
+      <c r="AN21" s="8"/>
+    </row>
+    <row r="22" spans="8:48">
+      <c r="AC22" s="5"/>
+      <c r="AN22" s="8"/>
+    </row>
+    <row r="23" spans="8:48">
+      <c r="AC23" s="5"/>
+      <c r="AN23" s="8"/>
+    </row>
+    <row r="24" spans="8:48">
+      <c r="AC24" s="5"/>
+      <c r="AN24" s="8"/>
+    </row>
+    <row r="25" spans="8:48">
+      <c r="AC25" s="5"/>
+      <c r="AN25" s="8"/>
+    </row>
+    <row r="26" spans="8:48">
+      <c r="AC26" s="5"/>
+      <c r="AN26" s="8"/>
+    </row>
+    <row r="27" spans="8:48">
+      <c r="AC27" s="5"/>
+      <c r="AN27" s="8"/>
+    </row>
+    <row r="28" spans="8:48">
+      <c r="AC28" s="5"/>
+      <c r="AN28" s="8"/>
+    </row>
+    <row r="29" spans="8:48">
+      <c r="AC29" s="5"/>
+      <c r="AN29" s="8"/>
+    </row>
+    <row r="30" spans="8:48">
+      <c r="AC30" s="5"/>
+      <c r="AN30" s="8"/>
+    </row>
+    <row r="31" spans="8:48">
+      <c r="AC31" s="5"/>
+      <c r="AN31" s="8"/>
+    </row>
+    <row r="32" spans="8:48">
+      <c r="AC32" s="5"/>
+      <c r="AN32" s="8"/>
+    </row>
+    <row r="33" spans="29:40">
+      <c r="AC33" s="5"/>
+      <c r="AN33" s="8"/>
+    </row>
+    <row r="34" spans="29:40">
+      <c r="AC34" s="5"/>
+      <c r="AN34" s="8"/>
+    </row>
+    <row r="35" spans="29:40">
+      <c r="AC35" s="5"/>
+      <c r="AN35" s="8"/>
+    </row>
+    <row r="36" spans="29:40">
+      <c r="AC36" s="5"/>
+      <c r="AN36" s="8"/>
+    </row>
+    <row r="37" spans="29:40">
+      <c r="AC37" s="5"/>
+      <c r="AN37" s="8"/>
+    </row>
+    <row r="38" spans="29:40">
+      <c r="AC38" s="5"/>
+      <c r="AN38" s="8"/>
+    </row>
+    <row r="39" spans="29:40">
+      <c r="AC39" s="5"/>
+      <c r="AN39" s="8"/>
+    </row>
+    <row r="40" spans="29:40">
+      <c r="AC40" s="5"/>
+      <c r="AN40" s="8"/>
+    </row>
+    <row r="41" spans="29:40">
+      <c r="AC41" s="5"/>
+      <c r="AN41" s="8"/>
+    </row>
+    <row r="42" spans="29:40">
+      <c r="AC42" s="5"/>
+      <c r="AN42" s="8"/>
+    </row>
+    <row r="43" spans="29:40">
+      <c r="AC43" s="5"/>
+      <c r="AN43" s="8"/>
+    </row>
+    <row r="44" spans="29:40">
+      <c r="AC44" s="5"/>
+      <c r="AN44" s="8"/>
+    </row>
+    <row r="45" spans="29:40">
+      <c r="AC45" s="5"/>
+      <c r="AN45" s="8"/>
+    </row>
+    <row r="46" spans="29:40">
+      <c r="AC46" s="5"/>
+      <c r="AN46" s="8"/>
+    </row>
+    <row r="47" spans="29:40">
+      <c r="AC47" s="5"/>
+      <c r="AN47" s="8"/>
+    </row>
+    <row r="48" spans="29:40">
+      <c r="AC48" s="5"/>
+      <c r="AN48" s="8"/>
+    </row>
+    <row r="49" spans="29:40">
+      <c r="AC49" s="5"/>
+      <c r="AN49" s="8"/>
+    </row>
+    <row r="50" spans="29:40">
+      <c r="AC50" s="5"/>
+      <c r="AN50" s="8"/>
+    </row>
+    <row r="51" spans="29:40">
+      <c r="AC51" s="5"/>
+      <c r="AN51" s="8"/>
+    </row>
+    <row r="52" spans="29:40">
+      <c r="AC52" s="5"/>
+      <c r="AN52" s="8"/>
+    </row>
+    <row r="53" spans="29:40">
+      <c r="AC53" s="5"/>
+      <c r="AN53" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AW53"/>
+  <autoFilter ref="A3:AV53"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update template master fleet
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/masterFleet.xlsx
+++ b/FMS.Website/files_upload/masterFleet.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AW$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AV$53</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -89,34 +89,12 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-data dari master data price list</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Gani, Ida:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
 Jika Restition = No, maka VAT = 10%* Monthly HMS Installment
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="AI3" authorId="0" shapeId="0">
+    <comment ref="AH3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ3" authorId="0" shapeId="0">
+    <comment ref="AP3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR3" authorId="0" shapeId="0">
+    <comment ref="AQ3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>MASTER DATA FLEET</t>
   </si>
@@ -331,9 +309,6 @@
   </si>
   <si>
     <t>Modified Date</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -697,13 +672,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW53"/>
+  <dimension ref="A1:AV53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="80" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -715,27 +690,28 @@
     <col min="17" max="17" width="14.42578125" customWidth="1"/>
     <col min="18" max="20" width="19.140625" customWidth="1"/>
     <col min="23" max="25" width="8.7109375" customWidth="1"/>
-    <col min="27" max="28" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="32" width="8.7109375" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" customWidth="1"/>
-    <col min="35" max="37" width="9.85546875" style="2" customWidth="1"/>
-    <col min="38" max="38" width="18" customWidth="1"/>
-    <col min="40" max="41" width="8.7109375" customWidth="1"/>
-    <col min="42" max="42" width="19" style="1" customWidth="1"/>
-    <col min="43" max="43" width="14.5703125" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" customWidth="1"/>
+    <col min="27" max="27" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11" customWidth="1"/>
+    <col min="30" max="31" width="8.7109375" customWidth="1"/>
+    <col min="32" max="32" width="11.7109375" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" customWidth="1"/>
+    <col min="34" max="36" width="9.85546875" style="2" customWidth="1"/>
+    <col min="37" max="37" width="18" customWidth="1"/>
+    <col min="39" max="40" width="8.7109375" customWidth="1"/>
+    <col min="41" max="41" width="19" style="1" customWidth="1"/>
+    <col min="42" max="42" width="14.5703125" customWidth="1"/>
+    <col min="43" max="43" width="13.5703125" customWidth="1"/>
+    <col min="48" max="48" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:48">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="15" customHeight="1"/>
-    <row r="3" spans="1:49">
+    <row r="2" spans="1:48" ht="15" customHeight="1"/>
+    <row r="3" spans="1:48">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -818,73 +794,70 @@
         <v>27</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AC3" t="s">
+        <v>29</v>
+      </c>
       <c r="AD3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE3" t="s">
         <v>30</v>
       </c>
+      <c r="AE3" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="AF3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="AI3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="AJ3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AK3" t="s">
         <v>37</v>
       </c>
+      <c r="AL3" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AM3" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AN3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AO3" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="AP3" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="AQ3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR3" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AR3" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="AS3" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AU3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AV3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49">
+    </row>
+    <row r="4" spans="1:48">
       <c r="H4" s="4"/>
       <c r="M4" s="4"/>
       <c r="P4" s="4"/>
@@ -895,23 +868,23 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="Z4" s="4"/>
+      <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AL4" s="7"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="10"/>
       <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
+      <c r="AR4" s="4"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
       <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-    </row>
-    <row r="5" spans="1:49">
+    </row>
+    <row r="5" spans="1:48">
       <c r="H5" s="4"/>
       <c r="M5" s="4"/>
       <c r="P5" s="4"/>
@@ -922,23 +895,23 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="Z5" s="4"/>
+      <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AL5" s="7"/>
       <c r="AM5" s="7"/>
       <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="10"/>
       <c r="AQ5" s="10"/>
-      <c r="AR5" s="10"/>
+      <c r="AR5" s="4"/>
       <c r="AS5" s="4"/>
       <c r="AT5" s="4"/>
       <c r="AU5" s="4"/>
       <c r="AV5" s="4"/>
-      <c r="AW5" s="4"/>
-    </row>
-    <row r="6" spans="1:49">
+    </row>
+    <row r="6" spans="1:48">
       <c r="H6" s="4"/>
       <c r="M6" s="4"/>
       <c r="P6" s="4"/>
@@ -949,23 +922,23 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="Z6" s="4"/>
+      <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="10"/>
       <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
+      <c r="AR6" s="4"/>
       <c r="AS6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
-      <c r="AW6" s="4"/>
-    </row>
-    <row r="7" spans="1:49">
+    </row>
+    <row r="7" spans="1:48">
       <c r="H7" s="4"/>
       <c r="M7" s="4"/>
       <c r="P7" s="4"/>
@@ -976,23 +949,23 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="Z7" s="4"/>
+      <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="10"/>
       <c r="AQ7" s="10"/>
-      <c r="AR7" s="10"/>
+      <c r="AR7" s="4"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
       <c r="AV7" s="4"/>
-      <c r="AW7" s="4"/>
-    </row>
-    <row r="8" spans="1:49">
+    </row>
+    <row r="8" spans="1:48">
       <c r="H8" s="4"/>
       <c r="M8" s="4"/>
       <c r="P8" s="4"/>
@@ -1003,23 +976,23 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="Z8" s="4"/>
+      <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="10"/>
       <c r="AQ8" s="10"/>
-      <c r="AR8" s="10"/>
+      <c r="AR8" s="4"/>
       <c r="AS8" s="4"/>
       <c r="AT8" s="4"/>
       <c r="AU8" s="4"/>
       <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-    </row>
-    <row r="9" spans="1:49">
+    </row>
+    <row r="9" spans="1:48">
       <c r="H9" s="4"/>
       <c r="M9" s="4"/>
       <c r="P9" s="4"/>
@@ -1030,23 +1003,23 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="Z9" s="4"/>
+      <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AL9" s="7"/>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="10"/>
       <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
+      <c r="AR9" s="4"/>
       <c r="AS9" s="4"/>
       <c r="AT9" s="4"/>
       <c r="AU9" s="4"/>
       <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-    </row>
-    <row r="10" spans="1:49">
+    </row>
+    <row r="10" spans="1:48">
       <c r="H10" s="4"/>
       <c r="M10" s="4"/>
       <c r="P10" s="4"/>
@@ -1057,23 +1030,23 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="Z10" s="4"/>
+      <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AL10" s="7"/>
       <c r="AM10" s="7"/>
       <c r="AN10" s="7"/>
-      <c r="AO10" s="7"/>
-      <c r="AP10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="10"/>
       <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
+      <c r="AR10" s="4"/>
       <c r="AS10" s="4"/>
       <c r="AT10" s="4"/>
       <c r="AU10" s="4"/>
       <c r="AV10" s="4"/>
-      <c r="AW10" s="4"/>
-    </row>
-    <row r="11" spans="1:49">
+    </row>
+    <row r="11" spans="1:48">
       <c r="H11" s="4"/>
       <c r="M11" s="4"/>
       <c r="P11" s="4"/>
@@ -1084,23 +1057,23 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="Z11" s="4"/>
+      <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AL11" s="7"/>
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="10"/>
       <c r="AQ11" s="10"/>
-      <c r="AR11" s="10"/>
+      <c r="AR11" s="4"/>
       <c r="AS11" s="4"/>
       <c r="AT11" s="4"/>
       <c r="AU11" s="4"/>
       <c r="AV11" s="4"/>
-      <c r="AW11" s="4"/>
-    </row>
-    <row r="12" spans="1:49">
+    </row>
+    <row r="12" spans="1:48">
       <c r="H12" s="4"/>
       <c r="M12" s="4"/>
       <c r="P12" s="4"/>
@@ -1111,23 +1084,23 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="Z12" s="4"/>
+      <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AL12" s="7"/>
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="10"/>
       <c r="AQ12" s="10"/>
-      <c r="AR12" s="10"/>
+      <c r="AR12" s="4"/>
       <c r="AS12" s="4"/>
       <c r="AT12" s="4"/>
       <c r="AU12" s="4"/>
       <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-    </row>
-    <row r="13" spans="1:49">
+    </row>
+    <row r="13" spans="1:48">
       <c r="H13" s="4"/>
       <c r="M13" s="4"/>
       <c r="P13" s="4"/>
@@ -1138,23 +1111,23 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="Z13" s="4"/>
+      <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AL13" s="7"/>
       <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="10"/>
       <c r="AQ13" s="10"/>
-      <c r="AR13" s="10"/>
+      <c r="AR13" s="4"/>
       <c r="AS13" s="4"/>
       <c r="AT13" s="4"/>
       <c r="AU13" s="4"/>
       <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-    </row>
-    <row r="14" spans="1:49">
+    </row>
+    <row r="14" spans="1:48">
       <c r="H14" s="4"/>
       <c r="M14" s="4"/>
       <c r="P14" s="4"/>
@@ -1165,23 +1138,23 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="Z14" s="4"/>
+      <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AL14" s="7"/>
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="9"/>
+      <c r="AO14" s="9"/>
+      <c r="AP14" s="10"/>
       <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
+      <c r="AR14" s="4"/>
       <c r="AS14" s="4"/>
       <c r="AT14" s="4"/>
       <c r="AU14" s="4"/>
       <c r="AV14" s="4"/>
-      <c r="AW14" s="4"/>
-    </row>
-    <row r="15" spans="1:49">
+    </row>
+    <row r="15" spans="1:48">
       <c r="H15" s="4"/>
       <c r="M15" s="4"/>
       <c r="P15" s="4"/>
@@ -1192,23 +1165,23 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="Z15" s="4"/>
+      <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AL15" s="7"/>
       <c r="AM15" s="7"/>
       <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="9"/>
+      <c r="AO15" s="9"/>
+      <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
-      <c r="AR15" s="10"/>
+      <c r="AR15" s="4"/>
       <c r="AS15" s="4"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
-      <c r="AW15" s="4"/>
-    </row>
-    <row r="16" spans="1:49">
+    </row>
+    <row r="16" spans="1:48">
       <c r="H16" s="4"/>
       <c r="M16" s="4"/>
       <c r="P16" s="4"/>
@@ -1219,23 +1192,23 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="Z16" s="4"/>
+      <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
-      <c r="AH16" s="4"/>
-      <c r="AI16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AL16" s="7"/>
       <c r="AM16" s="7"/>
       <c r="AN16" s="7"/>
-      <c r="AO16" s="7"/>
-      <c r="AP16" s="9"/>
+      <c r="AO16" s="9"/>
+      <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
-      <c r="AR16" s="10"/>
+      <c r="AR16" s="4"/>
       <c r="AS16" s="4"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
-      <c r="AW16" s="4"/>
-    </row>
-    <row r="17" spans="8:49">
+    </row>
+    <row r="17" spans="8:48">
       <c r="H17" s="4"/>
       <c r="M17" s="4"/>
       <c r="P17" s="4"/>
@@ -1246,23 +1219,23 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
       <c r="Z17" s="4"/>
+      <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AL17" s="7"/>
       <c r="AM17" s="7"/>
       <c r="AN17" s="7"/>
-      <c r="AO17" s="7"/>
-      <c r="AP17" s="9"/>
+      <c r="AO17" s="9"/>
+      <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
-      <c r="AR17" s="10"/>
+      <c r="AR17" s="4"/>
       <c r="AS17" s="4"/>
       <c r="AT17" s="4"/>
       <c r="AU17" s="4"/>
       <c r="AV17" s="4"/>
-      <c r="AW17" s="4"/>
-    </row>
-    <row r="18" spans="8:49">
+    </row>
+    <row r="18" spans="8:48">
       <c r="H18" s="4"/>
       <c r="M18" s="4"/>
       <c r="P18" s="4"/>
@@ -1273,23 +1246,23 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="Z18" s="4"/>
+      <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AL18" s="7"/>
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
-      <c r="AO18" s="7"/>
-      <c r="AP18" s="9"/>
+      <c r="AO18" s="9"/>
+      <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
-      <c r="AR18" s="10"/>
+      <c r="AR18" s="4"/>
       <c r="AS18" s="4"/>
       <c r="AT18" s="4"/>
       <c r="AU18" s="4"/>
       <c r="AV18" s="4"/>
-      <c r="AW18" s="4"/>
-    </row>
-    <row r="19" spans="8:49">
+    </row>
+    <row r="19" spans="8:48">
       <c r="H19" s="4"/>
       <c r="M19" s="4"/>
       <c r="P19" s="4"/>
@@ -1300,160 +1273,160 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="Z19" s="4"/>
+      <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AL19" s="7"/>
       <c r="AM19" s="7"/>
       <c r="AN19" s="7"/>
-      <c r="AO19" s="7"/>
-      <c r="AP19" s="9"/>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="10"/>
       <c r="AQ19" s="10"/>
-      <c r="AR19" s="10"/>
+      <c r="AR19" s="4"/>
       <c r="AS19" s="4"/>
       <c r="AT19" s="4"/>
       <c r="AU19" s="4"/>
       <c r="AV19" s="4"/>
-      <c r="AW19" s="4"/>
-    </row>
-    <row r="20" spans="8:49">
-      <c r="AD20" s="5"/>
-      <c r="AO20" s="8"/>
-    </row>
-    <row r="21" spans="8:49">
-      <c r="AD21" s="5"/>
-      <c r="AO21" s="8"/>
-    </row>
-    <row r="22" spans="8:49">
-      <c r="AD22" s="5"/>
-      <c r="AO22" s="8"/>
-    </row>
-    <row r="23" spans="8:49">
-      <c r="AD23" s="5"/>
-      <c r="AO23" s="8"/>
-    </row>
-    <row r="24" spans="8:49">
-      <c r="AD24" s="5"/>
-      <c r="AO24" s="8"/>
-    </row>
-    <row r="25" spans="8:49">
-      <c r="AD25" s="5"/>
-      <c r="AO25" s="8"/>
-    </row>
-    <row r="26" spans="8:49">
-      <c r="AD26" s="5"/>
-      <c r="AO26" s="8"/>
-    </row>
-    <row r="27" spans="8:49">
-      <c r="AD27" s="5"/>
-      <c r="AO27" s="8"/>
-    </row>
-    <row r="28" spans="8:49">
-      <c r="AD28" s="5"/>
-      <c r="AO28" s="8"/>
-    </row>
-    <row r="29" spans="8:49">
-      <c r="AD29" s="5"/>
-      <c r="AO29" s="8"/>
-    </row>
-    <row r="30" spans="8:49">
-      <c r="AD30" s="5"/>
-      <c r="AO30" s="8"/>
-    </row>
-    <row r="31" spans="8:49">
-      <c r="AD31" s="5"/>
-      <c r="AO31" s="8"/>
-    </row>
-    <row r="32" spans="8:49">
-      <c r="AD32" s="5"/>
-      <c r="AO32" s="8"/>
-    </row>
-    <row r="33" spans="30:41">
-      <c r="AD33" s="5"/>
-      <c r="AO33" s="8"/>
-    </row>
-    <row r="34" spans="30:41">
-      <c r="AD34" s="5"/>
-      <c r="AO34" s="8"/>
-    </row>
-    <row r="35" spans="30:41">
-      <c r="AD35" s="5"/>
-      <c r="AO35" s="8"/>
-    </row>
-    <row r="36" spans="30:41">
-      <c r="AD36" s="5"/>
-      <c r="AO36" s="8"/>
-    </row>
-    <row r="37" spans="30:41">
-      <c r="AD37" s="5"/>
-      <c r="AO37" s="8"/>
-    </row>
-    <row r="38" spans="30:41">
-      <c r="AD38" s="5"/>
-      <c r="AO38" s="8"/>
-    </row>
-    <row r="39" spans="30:41">
-      <c r="AD39" s="5"/>
-      <c r="AO39" s="8"/>
-    </row>
-    <row r="40" spans="30:41">
-      <c r="AD40" s="5"/>
-      <c r="AO40" s="8"/>
-    </row>
-    <row r="41" spans="30:41">
-      <c r="AD41" s="5"/>
-      <c r="AO41" s="8"/>
-    </row>
-    <row r="42" spans="30:41">
-      <c r="AD42" s="5"/>
-      <c r="AO42" s="8"/>
-    </row>
-    <row r="43" spans="30:41">
-      <c r="AD43" s="5"/>
-      <c r="AO43" s="8"/>
-    </row>
-    <row r="44" spans="30:41">
-      <c r="AD44" s="5"/>
-      <c r="AO44" s="8"/>
-    </row>
-    <row r="45" spans="30:41">
-      <c r="AD45" s="5"/>
-      <c r="AO45" s="8"/>
-    </row>
-    <row r="46" spans="30:41">
-      <c r="AD46" s="5"/>
-      <c r="AO46" s="8"/>
-    </row>
-    <row r="47" spans="30:41">
-      <c r="AD47" s="5"/>
-      <c r="AO47" s="8"/>
-    </row>
-    <row r="48" spans="30:41">
-      <c r="AD48" s="5"/>
-      <c r="AO48" s="8"/>
-    </row>
-    <row r="49" spans="30:41">
-      <c r="AD49" s="5"/>
-      <c r="AO49" s="8"/>
-    </row>
-    <row r="50" spans="30:41">
-      <c r="AD50" s="5"/>
-      <c r="AO50" s="8"/>
-    </row>
-    <row r="51" spans="30:41">
-      <c r="AD51" s="5"/>
-      <c r="AO51" s="8"/>
-    </row>
-    <row r="52" spans="30:41">
-      <c r="AD52" s="5"/>
-      <c r="AO52" s="8"/>
-    </row>
-    <row r="53" spans="30:41">
-      <c r="AD53" s="5"/>
-      <c r="AO53" s="8"/>
+    </row>
+    <row r="20" spans="8:48">
+      <c r="AC20" s="5"/>
+      <c r="AN20" s="8"/>
+    </row>
+    <row r="21" spans="8:48">
+      <c r="AC21" s="5"/>
+      <c r="AN21" s="8"/>
+    </row>
+    <row r="22" spans="8:48">
+      <c r="AC22" s="5"/>
+      <c r="AN22" s="8"/>
+    </row>
+    <row r="23" spans="8:48">
+      <c r="AC23" s="5"/>
+      <c r="AN23" s="8"/>
+    </row>
+    <row r="24" spans="8:48">
+      <c r="AC24" s="5"/>
+      <c r="AN24" s="8"/>
+    </row>
+    <row r="25" spans="8:48">
+      <c r="AC25" s="5"/>
+      <c r="AN25" s="8"/>
+    </row>
+    <row r="26" spans="8:48">
+      <c r="AC26" s="5"/>
+      <c r="AN26" s="8"/>
+    </row>
+    <row r="27" spans="8:48">
+      <c r="AC27" s="5"/>
+      <c r="AN27" s="8"/>
+    </row>
+    <row r="28" spans="8:48">
+      <c r="AC28" s="5"/>
+      <c r="AN28" s="8"/>
+    </row>
+    <row r="29" spans="8:48">
+      <c r="AC29" s="5"/>
+      <c r="AN29" s="8"/>
+    </row>
+    <row r="30" spans="8:48">
+      <c r="AC30" s="5"/>
+      <c r="AN30" s="8"/>
+    </row>
+    <row r="31" spans="8:48">
+      <c r="AC31" s="5"/>
+      <c r="AN31" s="8"/>
+    </row>
+    <row r="32" spans="8:48">
+      <c r="AC32" s="5"/>
+      <c r="AN32" s="8"/>
+    </row>
+    <row r="33" spans="29:40">
+      <c r="AC33" s="5"/>
+      <c r="AN33" s="8"/>
+    </row>
+    <row r="34" spans="29:40">
+      <c r="AC34" s="5"/>
+      <c r="AN34" s="8"/>
+    </row>
+    <row r="35" spans="29:40">
+      <c r="AC35" s="5"/>
+      <c r="AN35" s="8"/>
+    </row>
+    <row r="36" spans="29:40">
+      <c r="AC36" s="5"/>
+      <c r="AN36" s="8"/>
+    </row>
+    <row r="37" spans="29:40">
+      <c r="AC37" s="5"/>
+      <c r="AN37" s="8"/>
+    </row>
+    <row r="38" spans="29:40">
+      <c r="AC38" s="5"/>
+      <c r="AN38" s="8"/>
+    </row>
+    <row r="39" spans="29:40">
+      <c r="AC39" s="5"/>
+      <c r="AN39" s="8"/>
+    </row>
+    <row r="40" spans="29:40">
+      <c r="AC40" s="5"/>
+      <c r="AN40" s="8"/>
+    </row>
+    <row r="41" spans="29:40">
+      <c r="AC41" s="5"/>
+      <c r="AN41" s="8"/>
+    </row>
+    <row r="42" spans="29:40">
+      <c r="AC42" s="5"/>
+      <c r="AN42" s="8"/>
+    </row>
+    <row r="43" spans="29:40">
+      <c r="AC43" s="5"/>
+      <c r="AN43" s="8"/>
+    </row>
+    <row r="44" spans="29:40">
+      <c r="AC44" s="5"/>
+      <c r="AN44" s="8"/>
+    </row>
+    <row r="45" spans="29:40">
+      <c r="AC45" s="5"/>
+      <c r="AN45" s="8"/>
+    </row>
+    <row r="46" spans="29:40">
+      <c r="AC46" s="5"/>
+      <c r="AN46" s="8"/>
+    </row>
+    <row r="47" spans="29:40">
+      <c r="AC47" s="5"/>
+      <c r="AN47" s="8"/>
+    </row>
+    <row r="48" spans="29:40">
+      <c r="AC48" s="5"/>
+      <c r="AN48" s="8"/>
+    </row>
+    <row r="49" spans="29:40">
+      <c r="AC49" s="5"/>
+      <c r="AN49" s="8"/>
+    </row>
+    <row r="50" spans="29:40">
+      <c r="AC50" s="5"/>
+      <c r="AN50" s="8"/>
+    </row>
+    <row r="51" spans="29:40">
+      <c r="AC51" s="5"/>
+      <c r="AN51" s="8"/>
+    </row>
+    <row r="52" spans="29:40">
+      <c r="AC52" s="5"/>
+      <c r="AN52" s="8"/>
+    </row>
+    <row r="53" spans="29:40">
+      <c r="AC53" s="5"/>
+      <c r="AN53" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AW53"/>
+  <autoFilter ref="A3:AV53"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
fix cr1 add new field to master fleet
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/masterFleet.xlsx
+++ b/FMS.Website/files_upload/masterFleet.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AV$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$3:$AW$38</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
   <si>
     <t>MASTER DATA FLEET</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Regional</t>
+  </si>
+  <si>
+    <t>Sales Code</t>
   </si>
   <si>
     <t>Created By</t>
@@ -392,13 +395,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -417,6 +420,105 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -425,53 +527,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,77 +550,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -576,13 +579,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,25 +741,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,139 +759,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,17 +788,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,32 +814,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -868,8 +845,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,19 +880,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -901,149 +904,148 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1363,14 +1365,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AV38"/>
+  <dimension ref="A1:AW38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="AS4" sqref="AS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1408,8 +1410,8 @@
     <col min="39" max="40" width="8.71428571428571" customWidth="1"/>
     <col min="41" max="41" width="28.5714285714286" style="2" customWidth="1"/>
     <col min="42" max="42" width="14.5714285714286" customWidth="1"/>
-    <col min="43" max="43" width="13.5714285714286" customWidth="1"/>
-    <col min="48" max="48" width="14.1428571428571" customWidth="1"/>
+    <col min="43" max="44" width="13.5714285714286" customWidth="1"/>
+    <col min="49" max="49" width="14.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1431,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:48">
+    <row r="3" s="1" customFormat="1" spans="1:49">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1561,7 +1563,7 @@
       <c r="AQ3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AR3" s="11" t="s">
         <v>45</v>
       </c>
       <c r="AS3" s="1" t="s">
@@ -1574,66 +1576,69 @@
         <v>48</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:48">
+        <v>49</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:49">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P4" s="5">
         <v>2012</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T4" s="5"/>
       <c r="U4" s="6">
@@ -1643,16 +1648,16 @@
         <v>43131</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA4" s="5">
         <v>5293000</v>
@@ -1661,10 +1666,10 @@
         <v>529300</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE4" s="5">
         <v>1</v>
@@ -1674,7 +1679,7 @@
       </c>
       <c r="AG4" s="5"/>
       <c r="AH4" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AI4" s="6">
         <v>41306</v>
@@ -1683,25 +1688,26 @@
         <v>43132</v>
       </c>
       <c r="AK4" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AL4" s="5"/>
       <c r="AM4" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5">
         <v>5822300</v>
       </c>
       <c r="AP4" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
-      <c r="AV4" s="12"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
     </row>
     <row r="5" spans="29:40">
       <c r="AC5" s="8"/>
@@ -1840,7 +1846,7 @@
       <c r="AN38" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AV38"/>
+  <autoFilter ref="A3:AW38"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>

</xml_diff>